<commit_message>
Driving backwards n such
</commit_message>
<xml_diff>
--- a/assets/Meshes/Base_Mesh_4.xlsx
+++ b/assets/Meshes/Base_Mesh_4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimLe\PycharmProjects\JIP_ApronSim\assets\Meshes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADD8585-5AF2-4FF4-B17B-FD35DB7FBCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A4BA30-C3E2-416D-B650-847C724C4C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -343,8 +343,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:GJ158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BU60" sqref="BU60"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="DT17" sqref="DT17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9825,136 +9825,136 @@
         <v>1</v>
       </c>
       <c r="BW17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CP17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CQ17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CR17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CS17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CT17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CU17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CV17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CW17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CX17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DA17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DK17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DL17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DM17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DN17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DO17" s="1">
         <v>1</v>
@@ -10403,55 +10403,55 @@
         <v>1</v>
       </c>
       <c r="BW18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CG18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN18" s="1">
         <v>0</v>
@@ -10484,55 +10484,55 @@
         <v>0</v>
       </c>
       <c r="CX18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DA18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DG18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DH18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DI18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DJ18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DK18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DL18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DM18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DN18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DO18" s="1">
         <v>1</v>
@@ -11011,25 +11011,25 @@
         <v>0</v>
       </c>
       <c r="CG19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CJ19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN19" s="1">
         <v>0</v>
@@ -11062,25 +11062,25 @@
         <v>0</v>
       </c>
       <c r="CX19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DA19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DC19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DD19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE19" s="1">
         <v>0</v>
@@ -11598,16 +11598,16 @@
         <v>0</v>
       </c>
       <c r="CJ20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CK20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CL20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CM20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN20" s="1">
         <v>0</v>
@@ -11640,16 +11640,16 @@
         <v>0</v>
       </c>
       <c r="CX20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CY20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DA20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB20" s="1">
         <v>0</v>

</xml_diff>